<commit_message>
update : data 최신화
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2193"/>
+  <dimension ref="A1:H2230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>5177000</v>
+        <v>5047000</v>
       </c>
       <c r="H2" t="n">
         <v>3619000</v>
@@ -513,7 +513,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>7742000</v>
+        <v>7760000</v>
       </c>
       <c r="H3" t="n">
         <v>6900000</v>
@@ -535,7 +535,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
-        <v>9172000</v>
+        <v>9320000</v>
       </c>
       <c r="H4" t="n">
         <v>8113000</v>
@@ -560,7 +560,7 @@
         <v>10120000</v>
       </c>
       <c r="H5" t="n">
-        <v>9320000</v>
+        <v>9345000</v>
       </c>
     </row>
     <row r="6">
@@ -608,7 +608,7 @@
         <v>12815000</v>
       </c>
       <c r="H7" t="n">
-        <v>12131000</v>
+        <v>12112000</v>
       </c>
     </row>
     <row r="8">
@@ -632,7 +632,7 @@
         <v>14028000</v>
       </c>
       <c r="H8" t="n">
-        <v>13401000</v>
+        <v>13535000</v>
       </c>
     </row>
     <row r="9">
@@ -653,10 +653,10 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>25230000</v>
+        <v>24802000</v>
       </c>
       <c r="H9" t="n">
-        <v>18275000</v>
+        <v>17954000</v>
       </c>
     </row>
     <row r="10">
@@ -677,10 +677,10 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>32511000</v>
+        <v>33913000</v>
       </c>
       <c r="H10" t="n">
-        <v>25387000</v>
+        <v>25230000</v>
       </c>
     </row>
     <row r="11">
@@ -755,10 +755,10 @@
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>54812000</v>
+        <v>48777000</v>
       </c>
       <c r="H13" t="n">
-        <v>45409000</v>
+        <v>45517000</v>
       </c>
     </row>
     <row r="14">
@@ -781,10 +781,10 @@
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>58807000</v>
+        <v>54410000</v>
       </c>
       <c r="H14" t="n">
-        <v>55031000</v>
+        <v>49070000</v>
       </c>
     </row>
     <row r="15">
@@ -807,10 +807,10 @@
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>74830000</v>
+        <v>58807000</v>
       </c>
       <c r="H15" t="n">
-        <v>65951000</v>
+        <v>55580000</v>
       </c>
     </row>
     <row r="16">
@@ -832,8 +832,12 @@
         <v>5043500</v>
       </c>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>74830000</v>
+      </c>
+      <c r="H16" t="n">
+        <v>66208000</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -53061,19 +53065,907 @@
         <v>35491000</v>
       </c>
       <c r="C2193" t="n">
-        <v>-0.0012382507</v>
+        <v>-0.0012101086</v>
       </c>
       <c r="D2193" t="n">
-        <v>35790600</v>
+        <v>35789800</v>
       </c>
       <c r="E2193" t="n">
-        <v>35965000</v>
+        <v>35964600</v>
       </c>
       <c r="F2193" t="n">
-        <v>35639100</v>
+        <v>35638950</v>
       </c>
       <c r="G2193" t="inlineStr"/>
       <c r="H2193" t="inlineStr"/>
+    </row>
+    <row r="2194">
+      <c r="A2194" t="inlineStr">
+        <is>
+          <t>2023-09-26</t>
+        </is>
+      </c>
+      <c r="B2194" t="n">
+        <v>35566000</v>
+      </c>
+      <c r="C2194" t="n">
+        <v>0.0021132118</v>
+      </c>
+      <c r="D2194" t="n">
+        <v>35700600</v>
+      </c>
+      <c r="E2194" t="n">
+        <v>35927400</v>
+      </c>
+      <c r="F2194" t="n">
+        <v>35665800</v>
+      </c>
+      <c r="G2194" t="inlineStr"/>
+      <c r="H2194" t="inlineStr"/>
+    </row>
+    <row r="2195">
+      <c r="A2195" t="inlineStr">
+        <is>
+          <t>2023-09-27</t>
+        </is>
+      </c>
+      <c r="B2195" t="n">
+        <v>35982000</v>
+      </c>
+      <c r="C2195" t="n">
+        <v>0.0116965641</v>
+      </c>
+      <c r="D2195" t="n">
+        <v>35706600</v>
+      </c>
+      <c r="E2195" t="n">
+        <v>35949800</v>
+      </c>
+      <c r="F2195" t="n">
+        <v>35684150</v>
+      </c>
+      <c r="G2195" t="inlineStr"/>
+      <c r="H2195" t="inlineStr"/>
+    </row>
+    <row r="2196">
+      <c r="A2196" t="inlineStr">
+        <is>
+          <t>2023-09-28</t>
+        </is>
+      </c>
+      <c r="B2196" t="n">
+        <v>36596000</v>
+      </c>
+      <c r="C2196" t="n">
+        <v>0.0170640876</v>
+      </c>
+      <c r="D2196" t="n">
+        <v>35833800</v>
+      </c>
+      <c r="E2196" t="n">
+        <v>36009400</v>
+      </c>
+      <c r="F2196" t="n">
+        <v>35749200</v>
+      </c>
+      <c r="G2196" t="inlineStr"/>
+      <c r="H2196" t="inlineStr"/>
+    </row>
+    <row r="2197">
+      <c r="A2197" t="inlineStr">
+        <is>
+          <t>2023-09-29</t>
+        </is>
+      </c>
+      <c r="B2197" t="n">
+        <v>36444000</v>
+      </c>
+      <c r="C2197" t="n">
+        <v>-0.0041534594</v>
+      </c>
+      <c r="D2197" t="n">
+        <v>36015800</v>
+      </c>
+      <c r="E2197" t="n">
+        <v>36003800</v>
+      </c>
+      <c r="F2197" t="n">
+        <v>35807400</v>
+      </c>
+      <c r="G2197" t="inlineStr"/>
+      <c r="H2197" t="inlineStr"/>
+    </row>
+    <row r="2198">
+      <c r="A2198" t="inlineStr">
+        <is>
+          <t>2023-09-30</t>
+        </is>
+      </c>
+      <c r="B2198" t="n">
+        <v>36600000</v>
+      </c>
+      <c r="C2198" t="n">
+        <v>0.00428054</v>
+      </c>
+      <c r="D2198" t="n">
+        <v>36237600</v>
+      </c>
+      <c r="E2198" t="n">
+        <v>36013700</v>
+      </c>
+      <c r="F2198" t="n">
+        <v>35877600</v>
+      </c>
+      <c r="G2198" t="inlineStr"/>
+      <c r="H2198" t="inlineStr"/>
+    </row>
+    <row r="2199">
+      <c r="A2199" t="inlineStr">
+        <is>
+          <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="B2199" t="n">
+        <v>37789000</v>
+      </c>
+      <c r="C2199" t="n">
+        <v>0.0324863388</v>
+      </c>
+      <c r="D2199" t="n">
+        <v>36682200</v>
+      </c>
+      <c r="E2199" t="n">
+        <v>36191400</v>
+      </c>
+      <c r="F2199" t="n">
+        <v>36050700</v>
+      </c>
+      <c r="G2199" t="inlineStr"/>
+      <c r="H2199" t="inlineStr"/>
+    </row>
+    <row r="2200">
+      <c r="A2200" t="inlineStr">
+        <is>
+          <t>2023-10-02</t>
+        </is>
+      </c>
+      <c r="B2200" t="n">
+        <v>37424000</v>
+      </c>
+      <c r="C2200" t="n">
+        <v>-0.009658895400000001</v>
+      </c>
+      <c r="D2200" t="n">
+        <v>36970600</v>
+      </c>
+      <c r="E2200" t="n">
+        <v>36338600</v>
+      </c>
+      <c r="F2200" t="n">
+        <v>36168050</v>
+      </c>
+      <c r="G2200" t="inlineStr"/>
+      <c r="H2200" t="inlineStr"/>
+    </row>
+    <row r="2201">
+      <c r="A2201" t="inlineStr">
+        <is>
+          <t>2023-10-03</t>
+        </is>
+      </c>
+      <c r="B2201" t="n">
+        <v>37197000</v>
+      </c>
+      <c r="C2201" t="n">
+        <v>-0.0060656263</v>
+      </c>
+      <c r="D2201" t="n">
+        <v>37090800</v>
+      </c>
+      <c r="E2201" t="n">
+        <v>36462300</v>
+      </c>
+      <c r="F2201" t="n">
+        <v>36253050</v>
+      </c>
+      <c r="G2201" t="inlineStr"/>
+      <c r="H2201" t="inlineStr"/>
+    </row>
+    <row r="2202">
+      <c r="A2202" t="inlineStr">
+        <is>
+          <t>2023-10-04</t>
+        </is>
+      </c>
+      <c r="B2202" t="n">
+        <v>37595000</v>
+      </c>
+      <c r="C2202" t="n">
+        <v>0.0106997876</v>
+      </c>
+      <c r="D2202" t="n">
+        <v>37321000</v>
+      </c>
+      <c r="E2202" t="n">
+        <v>36668400</v>
+      </c>
+      <c r="F2202" t="n">
+        <v>36338350</v>
+      </c>
+      <c r="G2202" t="inlineStr"/>
+      <c r="H2202" t="inlineStr"/>
+    </row>
+    <row r="2203">
+      <c r="A2203" t="inlineStr">
+        <is>
+          <t>2023-10-05</t>
+        </is>
+      </c>
+      <c r="B2203" t="n">
+        <v>37258000</v>
+      </c>
+      <c r="C2203" t="n">
+        <v>-0.008963957999999999</v>
+      </c>
+      <c r="D2203" t="n">
+        <v>37452600</v>
+      </c>
+      <c r="E2203" t="n">
+        <v>36845100</v>
+      </c>
+      <c r="F2203" t="n">
+        <v>36404850</v>
+      </c>
+      <c r="G2203" t="inlineStr"/>
+      <c r="H2203" t="inlineStr"/>
+    </row>
+    <row r="2204">
+      <c r="A2204" t="inlineStr">
+        <is>
+          <t>2023-10-06</t>
+        </is>
+      </c>
+      <c r="B2204" t="n">
+        <v>37798000</v>
+      </c>
+      <c r="C2204" t="n">
+        <v>0.0144935316</v>
+      </c>
+      <c r="D2204" t="n">
+        <v>37454400</v>
+      </c>
+      <c r="E2204" t="n">
+        <v>37068300</v>
+      </c>
+      <c r="F2204" t="n">
+        <v>36497850</v>
+      </c>
+      <c r="G2204" t="inlineStr"/>
+      <c r="H2204" t="inlineStr"/>
+    </row>
+    <row r="2205">
+      <c r="A2205" t="inlineStr">
+        <is>
+          <t>2023-10-07</t>
+        </is>
+      </c>
+      <c r="B2205" t="n">
+        <v>37902000</v>
+      </c>
+      <c r="C2205" t="n">
+        <v>0.0027514683</v>
+      </c>
+      <c r="D2205" t="n">
+        <v>37550000</v>
+      </c>
+      <c r="E2205" t="n">
+        <v>37260300</v>
+      </c>
+      <c r="F2205" t="n">
+        <v>36605050</v>
+      </c>
+      <c r="G2205" t="inlineStr"/>
+      <c r="H2205" t="inlineStr"/>
+    </row>
+    <row r="2206">
+      <c r="A2206" t="inlineStr">
+        <is>
+          <t>2023-10-08</t>
+        </is>
+      </c>
+      <c r="B2206" t="n">
+        <v>37929000</v>
+      </c>
+      <c r="C2206" t="n">
+        <v>0.0007123635</v>
+      </c>
+      <c r="D2206" t="n">
+        <v>37696400</v>
+      </c>
+      <c r="E2206" t="n">
+        <v>37393600</v>
+      </c>
+      <c r="F2206" t="n">
+        <v>36701500</v>
+      </c>
+      <c r="G2206" t="inlineStr"/>
+      <c r="H2206" t="inlineStr"/>
+    </row>
+    <row r="2207">
+      <c r="A2207" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="B2207" t="n">
+        <v>37595000</v>
+      </c>
+      <c r="C2207" t="n">
+        <v>-0.0088059269</v>
+      </c>
+      <c r="D2207" t="n">
+        <v>37696400</v>
+      </c>
+      <c r="E2207" t="n">
+        <v>37508700</v>
+      </c>
+      <c r="F2207" t="n">
+        <v>36756250</v>
+      </c>
+      <c r="G2207" t="inlineStr"/>
+      <c r="H2207" t="inlineStr"/>
+    </row>
+    <row r="2208">
+      <c r="A2208" t="inlineStr">
+        <is>
+          <t>2023-10-10</t>
+        </is>
+      </c>
+      <c r="B2208" t="n">
+        <v>37336000</v>
+      </c>
+      <c r="C2208" t="n">
+        <v>-0.006889214</v>
+      </c>
+      <c r="D2208" t="n">
+        <v>37712000</v>
+      </c>
+      <c r="E2208" t="n">
+        <v>37582300</v>
+      </c>
+      <c r="F2208" t="n">
+        <v>36798000</v>
+      </c>
+      <c r="G2208" t="inlineStr"/>
+      <c r="H2208" t="inlineStr"/>
+    </row>
+    <row r="2209">
+      <c r="A2209" t="inlineStr">
+        <is>
+          <t>2023-10-11</t>
+        </is>
+      </c>
+      <c r="B2209" t="n">
+        <v>36671000</v>
+      </c>
+      <c r="C2209" t="n">
+        <v>-0.0178112278</v>
+      </c>
+      <c r="D2209" t="n">
+        <v>37486600</v>
+      </c>
+      <c r="E2209" t="n">
+        <v>37470500</v>
+      </c>
+      <c r="F2209" t="n">
+        <v>36830950</v>
+      </c>
+      <c r="G2209" t="inlineStr"/>
+      <c r="H2209" t="inlineStr"/>
+    </row>
+    <row r="2210">
+      <c r="A2210" t="inlineStr">
+        <is>
+          <t>2023-10-12</t>
+        </is>
+      </c>
+      <c r="B2210" t="n">
+        <v>36750000</v>
+      </c>
+      <c r="C2210" t="n">
+        <v>0.0021542909</v>
+      </c>
+      <c r="D2210" t="n">
+        <v>37256200</v>
+      </c>
+      <c r="E2210" t="n">
+        <v>37403100</v>
+      </c>
+      <c r="F2210" t="n">
+        <v>36870850</v>
+      </c>
+      <c r="G2210" t="inlineStr"/>
+      <c r="H2210" t="inlineStr"/>
+    </row>
+    <row r="2211">
+      <c r="A2211" t="inlineStr">
+        <is>
+          <t>2023-10-13</t>
+        </is>
+      </c>
+      <c r="B2211" t="n">
+        <v>36968000</v>
+      </c>
+      <c r="C2211" t="n">
+        <v>0.0059319728</v>
+      </c>
+      <c r="D2211" t="n">
+        <v>37064000</v>
+      </c>
+      <c r="E2211" t="n">
+        <v>37380200</v>
+      </c>
+      <c r="F2211" t="n">
+        <v>36921250</v>
+      </c>
+      <c r="G2211" t="inlineStr"/>
+      <c r="H2211" t="inlineStr"/>
+    </row>
+    <row r="2212">
+      <c r="A2212" t="inlineStr">
+        <is>
+          <t>2023-10-14</t>
+        </is>
+      </c>
+      <c r="B2212" t="n">
+        <v>36790000</v>
+      </c>
+      <c r="C2212" t="n">
+        <v>-0.0048149751</v>
+      </c>
+      <c r="D2212" t="n">
+        <v>36903000</v>
+      </c>
+      <c r="E2212" t="n">
+        <v>37299700</v>
+      </c>
+      <c r="F2212" t="n">
+        <v>36984050</v>
+      </c>
+      <c r="G2212" t="inlineStr"/>
+      <c r="H2212" t="inlineStr"/>
+    </row>
+    <row r="2213">
+      <c r="A2213" t="inlineStr">
+        <is>
+          <t>2023-10-15</t>
+        </is>
+      </c>
+      <c r="B2213" t="n">
+        <v>37086000</v>
+      </c>
+      <c r="C2213" t="n">
+        <v>0.0080456646</v>
+      </c>
+      <c r="D2213" t="n">
+        <v>36853000</v>
+      </c>
+      <c r="E2213" t="n">
+        <v>37282500</v>
+      </c>
+      <c r="F2213" t="n">
+        <v>37063800</v>
+      </c>
+      <c r="G2213" t="inlineStr"/>
+      <c r="H2213" t="inlineStr"/>
+    </row>
+    <row r="2214">
+      <c r="A2214" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
+      <c r="B2214" t="n">
+        <v>38697000</v>
+      </c>
+      <c r="C2214" t="n">
+        <v>0.0434395729</v>
+      </c>
+      <c r="D2214" t="n">
+        <v>37258200</v>
+      </c>
+      <c r="E2214" t="n">
+        <v>37372400</v>
+      </c>
+      <c r="F2214" t="n">
+        <v>37220350</v>
+      </c>
+      <c r="G2214" t="inlineStr"/>
+      <c r="H2214" t="inlineStr"/>
+    </row>
+    <row r="2215">
+      <c r="A2215" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
+      <c r="B2215" t="n">
+        <v>38652000</v>
+      </c>
+      <c r="C2215" t="n">
+        <v>-0.0011628808</v>
+      </c>
+      <c r="D2215" t="n">
+        <v>37638600</v>
+      </c>
+      <c r="E2215" t="n">
+        <v>37447400</v>
+      </c>
+      <c r="F2215" t="n">
+        <v>37353850</v>
+      </c>
+      <c r="G2215" t="inlineStr"/>
+      <c r="H2215" t="inlineStr"/>
+    </row>
+    <row r="2216">
+      <c r="A2216" t="inlineStr">
+        <is>
+          <t>2023-10-18</t>
+        </is>
+      </c>
+      <c r="B2216" t="n">
+        <v>38710000</v>
+      </c>
+      <c r="C2216" t="n">
+        <v>0.0015005692</v>
+      </c>
+      <c r="D2216" t="n">
+        <v>37987000</v>
+      </c>
+      <c r="E2216" t="n">
+        <v>37525500</v>
+      </c>
+      <c r="F2216" t="n">
+        <v>37459550</v>
+      </c>
+      <c r="G2216" t="inlineStr"/>
+      <c r="H2216" t="inlineStr"/>
+    </row>
+    <row r="2217">
+      <c r="A2217" t="inlineStr">
+        <is>
+          <t>2023-10-19</t>
+        </is>
+      </c>
+      <c r="B2217" t="n">
+        <v>39000000</v>
+      </c>
+      <c r="C2217" t="n">
+        <v>0.0074916042</v>
+      </c>
+      <c r="D2217" t="n">
+        <v>38429000</v>
+      </c>
+      <c r="E2217" t="n">
+        <v>37666000</v>
+      </c>
+      <c r="F2217" t="n">
+        <v>37587350</v>
+      </c>
+      <c r="G2217" t="inlineStr"/>
+      <c r="H2217" t="inlineStr"/>
+    </row>
+    <row r="2218">
+      <c r="A2218" t="inlineStr">
+        <is>
+          <t>2023-10-20</t>
+        </is>
+      </c>
+      <c r="B2218" t="n">
+        <v>40250000</v>
+      </c>
+      <c r="C2218" t="n">
+        <v>0.0320512821</v>
+      </c>
+      <c r="D2218" t="n">
+        <v>39061800</v>
+      </c>
+      <c r="E2218" t="n">
+        <v>37957400</v>
+      </c>
+      <c r="F2218" t="n">
+        <v>37769850</v>
+      </c>
+      <c r="G2218" t="inlineStr"/>
+      <c r="H2218" t="inlineStr"/>
+    </row>
+    <row r="2219">
+      <c r="A2219" t="inlineStr">
+        <is>
+          <t>2023-10-21</t>
+        </is>
+      </c>
+      <c r="B2219" t="n">
+        <v>40400000</v>
+      </c>
+      <c r="C2219" t="n">
+        <v>0.0037267081</v>
+      </c>
+      <c r="D2219" t="n">
+        <v>39402400</v>
+      </c>
+      <c r="E2219" t="n">
+        <v>38330300</v>
+      </c>
+      <c r="F2219" t="n">
+        <v>37900400</v>
+      </c>
+      <c r="G2219" t="inlineStr"/>
+      <c r="H2219" t="inlineStr"/>
+    </row>
+    <row r="2220">
+      <c r="A2220" t="inlineStr">
+        <is>
+          <t>2023-10-22</t>
+        </is>
+      </c>
+      <c r="B2220" t="n">
+        <v>40354000</v>
+      </c>
+      <c r="C2220" t="n">
+        <v>-0.0011386139</v>
+      </c>
+      <c r="D2220" t="n">
+        <v>39742800</v>
+      </c>
+      <c r="E2220" t="n">
+        <v>38690700</v>
+      </c>
+      <c r="F2220" t="n">
+        <v>38046900</v>
+      </c>
+      <c r="G2220" t="inlineStr"/>
+      <c r="H2220" t="inlineStr"/>
+    </row>
+    <row r="2221">
+      <c r="A2221" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
+      <c r="B2221" t="n">
+        <v>44179000</v>
+      </c>
+      <c r="C2221" t="n">
+        <v>0.0947861426</v>
+      </c>
+      <c r="D2221" t="n">
+        <v>40836600</v>
+      </c>
+      <c r="E2221" t="n">
+        <v>39411800</v>
+      </c>
+      <c r="F2221" t="n">
+        <v>38396000</v>
+      </c>
+      <c r="G2221" t="inlineStr"/>
+      <c r="H2221" t="inlineStr"/>
+    </row>
+    <row r="2222">
+      <c r="A2222" t="inlineStr">
+        <is>
+          <t>2023-10-24</t>
+        </is>
+      </c>
+      <c r="B2222" t="n">
+        <v>45599000</v>
+      </c>
+      <c r="C2222" t="n">
+        <v>0.0321419679</v>
+      </c>
+      <c r="D2222" t="n">
+        <v>42156400</v>
+      </c>
+      <c r="E2222" t="n">
+        <v>40292700</v>
+      </c>
+      <c r="F2222" t="n">
+        <v>38796200</v>
+      </c>
+      <c r="G2222" t="inlineStr"/>
+      <c r="H2222" t="inlineStr"/>
+    </row>
+    <row r="2223">
+      <c r="A2223" t="inlineStr">
+        <is>
+          <t>2023-10-25</t>
+        </is>
+      </c>
+      <c r="B2223" t="n">
+        <v>46484000</v>
+      </c>
+      <c r="C2223" t="n">
+        <v>0.0194083204</v>
+      </c>
+      <c r="D2223" t="n">
+        <v>43403200</v>
+      </c>
+      <c r="E2223" t="n">
+        <v>41232500</v>
+      </c>
+      <c r="F2223" t="n">
+        <v>39257500</v>
+      </c>
+      <c r="G2223" t="inlineStr"/>
+      <c r="H2223" t="inlineStr"/>
+    </row>
+    <row r="2224">
+      <c r="A2224" t="inlineStr">
+        <is>
+          <t>2023-10-26</t>
+        </is>
+      </c>
+      <c r="B2224" t="n">
+        <v>46141000</v>
+      </c>
+      <c r="C2224" t="n">
+        <v>-0.0073788831</v>
+      </c>
+      <c r="D2224" t="n">
+        <v>44551400</v>
+      </c>
+      <c r="E2224" t="n">
+        <v>41976900</v>
+      </c>
+      <c r="F2224" t="n">
+        <v>39674650</v>
+      </c>
+      <c r="G2224" t="inlineStr"/>
+      <c r="H2224" t="inlineStr"/>
+    </row>
+    <row r="2225">
+      <c r="A2225" t="inlineStr">
+        <is>
+          <t>2023-10-27</t>
+        </is>
+      </c>
+      <c r="B2225" t="n">
+        <v>45980000</v>
+      </c>
+      <c r="C2225" t="n">
+        <v>-0.0034893045</v>
+      </c>
+      <c r="D2225" t="n">
+        <v>45676600</v>
+      </c>
+      <c r="E2225" t="n">
+        <v>42709700</v>
+      </c>
+      <c r="F2225" t="n">
+        <v>40078550</v>
+      </c>
+      <c r="G2225" t="inlineStr"/>
+      <c r="H2225" t="inlineStr"/>
+    </row>
+    <row r="2226">
+      <c r="A2226" t="inlineStr">
+        <is>
+          <t>2023-10-28</t>
+        </is>
+      </c>
+      <c r="B2226" t="n">
+        <v>46314000</v>
+      </c>
+      <c r="C2226" t="n">
+        <v>0.0072640278</v>
+      </c>
+      <c r="D2226" t="n">
+        <v>46103600</v>
+      </c>
+      <c r="E2226" t="n">
+        <v>43470100</v>
+      </c>
+      <c r="F2226" t="n">
+        <v>40497800</v>
+      </c>
+      <c r="G2226" t="inlineStr"/>
+      <c r="H2226" t="inlineStr"/>
+    </row>
+    <row r="2227">
+      <c r="A2227" t="inlineStr">
+        <is>
+          <t>2023-10-29</t>
+        </is>
+      </c>
+      <c r="B2227" t="n">
+        <v>46825000</v>
+      </c>
+      <c r="C2227" t="n">
+        <v>0.0110333808</v>
+      </c>
+      <c r="D2227" t="n">
+        <v>46348800</v>
+      </c>
+      <c r="E2227" t="n">
+        <v>44252600</v>
+      </c>
+      <c r="F2227" t="n">
+        <v>40959300</v>
+      </c>
+      <c r="G2227" t="inlineStr"/>
+      <c r="H2227" t="inlineStr"/>
+    </row>
+    <row r="2228">
+      <c r="A2228" t="inlineStr">
+        <is>
+          <t>2023-10-30</t>
+        </is>
+      </c>
+      <c r="B2228" t="n">
+        <v>46732000</v>
+      </c>
+      <c r="C2228" t="n">
+        <v>-0.0019861185</v>
+      </c>
+      <c r="D2228" t="n">
+        <v>46398400</v>
+      </c>
+      <c r="E2228" t="n">
+        <v>44900800</v>
+      </c>
+      <c r="F2228" t="n">
+        <v>41429100</v>
+      </c>
+      <c r="G2228" t="inlineStr"/>
+      <c r="H2228" t="inlineStr"/>
+    </row>
+    <row r="2229">
+      <c r="A2229" t="inlineStr">
+        <is>
+          <t>2023-10-31</t>
+        </is>
+      </c>
+      <c r="B2229" t="n">
+        <v>47030000</v>
+      </c>
+      <c r="C2229" t="n">
+        <v>0.0063767868</v>
+      </c>
+      <c r="D2229" t="n">
+        <v>46576200</v>
+      </c>
+      <c r="E2229" t="n">
+        <v>45563800</v>
+      </c>
+      <c r="F2229" t="n">
+        <v>41947050</v>
+      </c>
+      <c r="G2229" t="inlineStr"/>
+      <c r="H2229" t="inlineStr"/>
+    </row>
+    <row r="2230">
+      <c r="A2230" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B2230" t="n">
+        <v>46972000</v>
+      </c>
+      <c r="C2230" t="n">
+        <v>-0.0012332554</v>
+      </c>
+      <c r="D2230" t="n">
+        <v>46777200</v>
+      </c>
+      <c r="E2230" t="n">
+        <v>46225100</v>
+      </c>
+      <c r="F2230" t="n">
+        <v>42458150</v>
+      </c>
+      <c r="G2230" t="inlineStr"/>
+      <c r="H2230" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>